<commit_message>
DateOfInspection is added. Site 7 and 8 interchanged.
</commit_message>
<xml_diff>
--- a/Testing_Results.xlsx
+++ b/Testing_Results.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DDAS" sheetId="2" r:id="rId1"/>
     <sheet name="DDAS Testing" sheetId="1" r:id="rId2"/>
+    <sheet name="DDAS_ICON" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DDAS!$A$1:$D$1148</definedName>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="108">
   <si>
     <t>URL</t>
   </si>
@@ -153,13 +154,6 @@
     <t>Search the names directly from the available list</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has a search box. 
-</t>
-  </si>
-  <si>
     <t>15 Sep 2016: Unable to test this site with PhantomJS driver. Exception - StaleElementReferenceException. Need to look into this</t>
   </si>
   <si>
@@ -179,9 +173,6 @@
     <t>Navigate to the website, Click on 'PHS administrative action bulletin board' link and search for names
 Alternate URL: https://ori.hhs.gov/ORI_PHS_alert.html?d=update
 27-Sep-16: Connected to mongodb. Able to add extracted records</t>
-  </si>
-  <si>
-    <t>Adding RowNumber is pending</t>
   </si>
   <si>
     <t>21-Sep-16: Need to find a way to bypass the search and download all records at once. Currently going with the web scraping option but need to internally make call to the SAM server ang get the details at one go
@@ -322,6 +313,64 @@
   </si>
   <si>
     <t>May have to include NCAGE code as well</t>
+  </si>
+  <si>
+    <t>Effective date</t>
+  </si>
+  <si>
+    <t>Insp. Date</t>
+  </si>
+  <si>
+    <t>Letter Issued</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Action Date</t>
+  </si>
+  <si>
+    <t>Date of status</t>
+  </si>
+  <si>
+    <t>Memo</t>
+  </si>
+  <si>
+    <t>Inspection start/end date</t>
+  </si>
+  <si>
+    <t>Excl. Date</t>
+  </si>
+  <si>
+    <t>Effective</t>
+  </si>
+  <si>
+    <t>Activation date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has a search box
+</t>
+  </si>
+  <si>
+    <t>Inspection Date Field Names</t>
+  </si>
+  <si>
+    <t>Sites</t>
+  </si>
+  <si>
+    <t>Column Name for Inspection Date</t>
+  </si>
+  <si>
+    <t>Start date was considered as the Inspection date in the template shared. The same will be taken up in the application as well</t>
+  </si>
+  <si>
+    <t>It appears that the Inspection date has been picked from 'Memo' column. It would be feasible if the date is read from a column dedicated for 'Inspection Date', similar to the rest of the sites. Let us know if the whole text can be taken up as 'Inspection Date'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are two fields with dates - Activation date and Expiration date. As per the template shared, it appears that 'Activation date' is taken up as 'Inspection date'. Let us know if this is correct </t>
+  </si>
+  <si>
+    <t>Unable to find out the inspection date in the given template for this site</t>
   </si>
 </sst>
 </file>
@@ -353,7 +402,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,12 +412,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,7 +468,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -457,15 +500,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -777,12 +827,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="61.5703125" style="13" customWidth="1"/>
-    <col min="3" max="4" width="19.42578125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="13"/>
-    <col min="6" max="6" width="31.7109375" style="13" customWidth="1"/>
-    <col min="7" max="16384" width="16.5703125" style="13"/>
+    <col min="1" max="1" width="43.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="61.5703125" style="12" customWidth="1"/>
+    <col min="3" max="4" width="19.42578125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="12"/>
+    <col min="6" max="6" width="31.7109375" style="12" customWidth="1"/>
+    <col min="7" max="16384" width="16.5703125" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -793,22 +843,22 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="H1" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -821,26 +871,26 @@
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>73</v>
+      <c r="D2" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H2" s="1">
         <v>153</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>90</v>
+      <c r="I2" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -854,16 +904,16 @@
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H3" s="1">
         <v>19960</v>
@@ -879,14 +929,14 @@
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>72</v>
+      <c r="D4" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1">
@@ -904,10 +954,10 @@
         <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -926,10 +976,10 @@
         <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -947,14 +997,14 @@
       <c r="C7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>77</v>
+      <c r="D7" s="11" t="s">
+        <v>74</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1">
@@ -972,13 +1022,13 @@
         <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -993,11 +1043,11 @@
       <c r="C9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>78</v>
+      <c r="D9" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1008,26 +1058,26 @@
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="12" t="s">
         <v>81</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="13" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1040,17 +1090,17 @@
       <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>83</v>
+      <c r="D11" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -1062,25 +1112,25 @@
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>91</v>
+        <v>62</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1093,7 +1143,7 @@
       <c r="C13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="11">
         <v>42684</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1101,10 +1151,10 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1129,10 +1179,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="F4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,9 +1196,10 @@
     <col min="7" max="7" width="26.85546875" customWidth="1"/>
     <col min="8" max="8" width="31.28515625" customWidth="1"/>
     <col min="9" max="9" width="32" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -1159,7 +1210,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
@@ -1168,7 +1219,7 @@
         <v>36</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>37</v>
@@ -1176,8 +1227,11 @@
       <c r="I1" s="10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J1" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1188,10 +1242,10 @@
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F2" s="1">
         <v>4</v>
@@ -1201,8 +1255,11 @@
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="J2" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1225,11 +1282,14 @@
         <v>34</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="J3" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1243,16 +1303,19 @@
         <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J4" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1274,8 +1337,11 @@
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1289,7 +1355,7 @@
         <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F6" s="1">
         <v>2</v>
@@ -1299,8 +1365,11 @@
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J6" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1314,7 +1383,7 @@
         <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F7" s="1">
         <v>7</v>
@@ -1324,8 +1393,11 @@
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J7" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1347,8 +1419,11 @@
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="J8" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1362,14 +1437,17 @@
         <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="9"/>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J9" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1392,13 +1470,14 @@
         <v>32</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1418,19 +1497,22 @@
       <c r="G11" s="1"/>
       <c r="H11" s="9"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+      <c r="J11" s="14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>43</v>
+      <c r="C12" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>41</v>
@@ -1438,13 +1520,16 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1470,8 +1555,9 @@
         <v>39</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="J13" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1491,4 +1577,150 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Error with downloading supporting documents is resolved
</commit_message>
<xml_diff>
--- a/Testing_Results.xlsx
+++ b/Testing_Results.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="105">
   <si>
     <t>URL</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>8. Clinical Investigator Inspection List (CBER)</t>
+  </si>
+  <si>
+    <t>https://www.accessdata.fda.gov/scripts/warningletters/wlSearchResultExcel.cfm?qryStr=</t>
   </si>
 </sst>
 </file>
@@ -504,8 +507,36 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1164,8 +1195,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,7 +1308,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>104</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
UI for 5 site sources was updated. PageMaps is changed to read last updated date. Tested OK.
</commit_message>
<xml_diff>
--- a/Testing_Results.xlsx
+++ b/Testing_Results.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DDAS" sheetId="2" r:id="rId1"/>
     <sheet name="DDAS Testing" sheetId="1" r:id="rId2"/>
+    <sheet name="Site Sources" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DDAS!$A$1:$D$1148</definedName>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="129">
   <si>
     <t>URL</t>
   </si>
@@ -361,6 +362,78 @@
   </si>
   <si>
     <t>https://www.accessdata.fda.gov/scripts/warningletters/wlSearchResultExcel.cfm?qryStr=</t>
+  </si>
+  <si>
+    <t>Site Updated (UI)</t>
+  </si>
+  <si>
+    <t>28 Jan 2019: UI updated. Changes made in webscraping.selenium/pageMaps to read page last updated date</t>
+  </si>
+  <si>
+    <t>No Changes</t>
+  </si>
+  <si>
+    <t>28 Jan 2019: UI updated. Changes do not affect the data extraction as page last updated element is not used beacause of file download, which happens every day.</t>
+  </si>
+  <si>
+    <t>Site unavailable</t>
+  </si>
+  <si>
+    <t>No changes</t>
+  </si>
+  <si>
+    <t>UI Changed (Y/N)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Action Carried</t>
+  </si>
+  <si>
+    <t>Code updated to reflect site last updated date</t>
+  </si>
+  <si>
+    <t>File is downloaded every day, hence site last updated is not read</t>
+  </si>
+  <si>
+    <t>Site unavalable</t>
+  </si>
+  <si>
+    <t>FDA Debarment List</t>
+  </si>
+  <si>
+    <t>Clinical Investigator Inspection List (CLIL)(CDER)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FDA Warning Letters and Responses </t>
+  </si>
+  <si>
+    <t>Notice of Opportunity for Hearing (NOOH) – Proposal to Debar</t>
+  </si>
+  <si>
+    <t>Adequate Assurances List for Clinical Investigators</t>
+  </si>
+  <si>
+    <t>Clinical Investigators – Disqualification Proceedings (FDA Disqualified/Restricted)</t>
+  </si>
+  <si>
+    <t>Clinical Investigator Inspection List (CBER)</t>
+  </si>
+  <si>
+    <t>PHS Administrative Actions Listing</t>
+  </si>
+  <si>
+    <t>HHS/OIG/ EXCLUSIONS DATABASE SEARCH/ FRAUD</t>
+  </si>
+  <si>
+    <t>HHS/OIG Corporate Integrity Agreements/Watch List</t>
+  </si>
+  <si>
+    <t>SAM/SYSTEM FOR AWARD MANAGEMENT</t>
+  </si>
+  <si>
+    <t>LIST OF SPECIALLY DESIGNATED NATIONALS</t>
   </si>
 </sst>
 </file>
@@ -406,7 +479,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -453,12 +526,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -501,6 +583,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -835,8 +926,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,10 +1284,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,7 +1304,7 @@
     <col min="10" max="10" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -1244,8 +1335,11 @@
       <c r="J1" s="8" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="L1" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1272,8 +1366,11 @@
       <c r="J2" s="14" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1302,8 +1399,11 @@
       <c r="J3" s="13" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1328,8 +1428,11 @@
       <c r="J4" s="14" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1354,8 +1457,11 @@
       <c r="J5" s="14" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1382,8 +1488,11 @@
       <c r="J6" s="14" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1410,8 +1519,11 @@
       <c r="J7" s="14" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>102</v>
       </c>
@@ -1434,8 +1546,11 @@
       <c r="J8" s="14" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>103</v>
       </c>
@@ -1461,7 +1576,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1491,7 +1606,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1515,7 +1630,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1543,7 +1658,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1590,4 +1705,164 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
caching is added for sitescandata.cs
</commit_message>
<xml_diff>
--- a/Testing_Results.xlsx
+++ b/Testing_Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="DDAS" sheetId="2" r:id="rId1"/>
@@ -13,6 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DDAS!$A$1:$D$1148</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Site Sources'!$A$1:$C$13</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -388,9 +389,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Action Carried</t>
-  </si>
-  <si>
     <t>Code updated to reflect site last updated date</t>
   </si>
   <si>
@@ -434,6 +432,9 @@
   </si>
   <si>
     <t>LIST OF SPECIALLY DESIGNATED NATIONALS</t>
+  </si>
+  <si>
+    <t>Action Carried Out</t>
   </si>
 </sst>
 </file>
@@ -926,8 +927,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,67 +1731,67 @@
         <v>111</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>112</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>112</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>55</v>
@@ -1801,18 +1802,18 @@
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>55</v>
@@ -1823,42 +1824,42 @@
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged with Development and version is changed to 1.1.3
</commit_message>
<xml_diff>
--- a/Testing_Results.xlsx
+++ b/Testing_Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DDAS" sheetId="2" r:id="rId1"/>
@@ -13,14 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DDAS!$A$1:$D$1148</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Site Sources'!$A$1:$C$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Site Sources'!$A$1:$D$13</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="132">
   <si>
     <t>URL</t>
   </si>
@@ -435,6 +435,15 @@
   </si>
   <si>
     <t>Action Carried Out</t>
+  </si>
+  <si>
+    <t>Working</t>
+  </si>
+  <si>
+    <t>Have to explore options to download file or to scrape the data similar to other sites</t>
+  </si>
+  <si>
+    <t>Not Working</t>
   </si>
 </sst>
 </file>
@@ -541,7 +550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -594,6 +603,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -927,8 +937,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,9 +1731,10 @@
     <col min="1" max="1" width="48" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="35.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>28</v>
       </c>
@@ -1733,8 +1744,11 @@
       <c r="C1" s="16" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D1" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>116</v>
       </c>
@@ -1744,8 +1758,11 @@
       <c r="C2" s="9" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D2" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>117</v>
       </c>
@@ -1755,19 +1772,23 @@
       <c r="C3" s="9" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D3" s="18"/>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>118</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>112</v>
+        <v>30</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>119</v>
       </c>
@@ -1777,8 +1798,11 @@
       <c r="C5" s="9" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>120</v>
       </c>
@@ -1788,8 +1812,9 @@
       <c r="C6" s="9" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>121</v>
       </c>
@@ -1799,8 +1824,9 @@
       <c r="C7" s="9" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" s="18"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>122</v>
       </c>
@@ -1810,8 +1836,11 @@
       <c r="C8" s="9" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>123</v>
       </c>
@@ -1821,8 +1850,9 @@
       <c r="C9" s="9" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D9" s="18"/>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>124</v>
       </c>
@@ -1832,8 +1862,11 @@
       <c r="C10" s="9" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D10" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>125</v>
       </c>
@@ -1843,8 +1876,11 @@
       <c r="C11" s="9" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D11" s="16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>126</v>
       </c>
@@ -1852,8 +1888,9 @@
       <c r="C12" s="9" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>127</v>
       </c>
@@ -1861,6 +1898,7 @@
       <c r="C13" s="9" t="s">
         <v>114</v>
       </c>
+      <c r="D13" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
version updated to T1.1.7
</commit_message>
<xml_diff>
--- a/Testing_Results.xlsx
+++ b/Testing_Results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="140">
   <si>
     <t>URL</t>
   </si>
@@ -435,6 +435,40 @@
   </si>
   <si>
     <t>Action Carried Out</t>
+  </si>
+  <si>
+    <t>James D. Hudson</t>
+  </si>
+  <si>
+    <t>Bhandari Ranjan</t>
+  </si>
+  <si>
+    <t>Bowling, Chetwynd E., MD</t>
+  </si>
+  <si>
+    <t>RIETMEIJER, CORNELIUS</t>
+  </si>
+  <si>
+    <t>Ramadugu Venkata Sudheer Kumar</t>
+  </si>
+  <si>
+    <t>Patrick Bell</t>
+  </si>
+  <si>
+    <t>Lowrey, Gerald</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+ROBBY LEMON OWENS</t>
+  </si>
+  <si>
+    <t>Coroniti, Lisa Marie</t>
+  </si>
+  <si>
+    <t>Williams Joseph</t>
+  </si>
+  <si>
+    <t>Zaydan Muhammad</t>
   </si>
 </sst>
 </file>
@@ -925,10 +959,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +975,7 @@
     <col min="7" max="16384" width="16.5703125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>28</v>
       </c>
@@ -967,7 +1001,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -998,8 +1032,11 @@
       <c r="J2" s="12" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1024,8 +1061,11 @@
       <c r="H3" s="1">
         <v>19960</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="K3" s="12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1048,8 +1088,11 @@
       <c r="H4" s="1">
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1070,8 +1113,11 @@
       <c r="H5" s="1">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1093,7 +1139,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1116,8 +1162,11 @@
       <c r="H7" s="1">
         <v>225</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1138,8 +1187,11 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1158,8 +1210,11 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1185,8 +1240,11 @@
       <c r="I10" s="12" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1209,8 +1267,11 @@
         <v>64</v>
       </c>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="K11" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1238,8 +1299,11 @@
       <c r="I12" s="12" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1261,6 +1325,9 @@
       </c>
       <c r="H13" s="1" t="s">
         <v>67</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1713,7 +1780,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>